<commit_message>
A sample CRUD app
</commit_message>
<xml_diff>
--- a/Delivery Plan_Wells Fargo-IIHT-Full Stack Engineering.xlsx
+++ b/Delivery Plan_Wells Fargo-IIHT-Full Stack Engineering.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="19200" windowHeight="7110"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="19200" windowHeight="7110"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery Plan" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Delivery Plan'!$B$1:$I$66</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1166,7 +1167,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9:F16"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>